<commit_message>
new updates and fix
</commit_message>
<xml_diff>
--- a/public/assets_v1/import_example/Users Example.xlsx
+++ b/public/assets_v1/import_example/Users Example.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programs\laragon\www\arabicArabs\public\assets_v1\import_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\arabicArabs\public\assets_v1\import_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB3A80-F773-4C9F-B445-3D7FB4447CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F0B27C-ED7A-4C4F-8C1E-D26188B7354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Email</t>
   </si>
@@ -43,9 +56,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Learning Years</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -56,9 +66,6 @@
   </si>
   <si>
     <t>Required Column</t>
-  </si>
-  <si>
-    <t>0 to 12</t>
   </si>
   <si>
     <t>1 or 0</t>
@@ -88,12 +95,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -155,8 +164,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ارتباط تشعبي" xfId="1" builtinId="8"/>
-    <cellStyle name="عادي" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -458,30 +467,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -499,113 +507,102 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="P2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="P3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P4" s="5" t="s">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="5" t="s">
+      <c r="P4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="P5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O10" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O11" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P7" s="5" t="s">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O14" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P10" s="4" t="s">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="O16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P11" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P13" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P16" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>